<commit_message>
deprecated 'eigs'; use 'eigenvalues_and_spectral_matrices' instead
</commit_message>
<xml_diff>
--- a/samples/samples.xlsx
+++ b/samples/samples.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DCPROGS\SCALCS\scalcs\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remigijus.lape\SCALCS\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C76B61-C46B-4007-92F6-4B7C4C002A95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F720B041-826C-4892-BD6C-601F12951666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8916" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28755" yWindow="30" windowWidth="11895" windowHeight="15510" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH82" sheetId="1" r:id="rId1"/>
     <sheet name="1cycle" sheetId="2" r:id="rId2"/>
+    <sheet name="GlyRa1b-gly" sheetId="3" r:id="rId3"/>
+    <sheet name="GlyRa1b-tau" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="90">
   <si>
     <t>mectitle</t>
   </si>
@@ -205,13 +207,109 @@
   </si>
   <si>
     <t>constrain</t>
+  </si>
+  <si>
+    <t>Burzomato2004 heteromericGlyR - glycine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 site flip </t>
+  </si>
+  <si>
+    <t>Burzomato a1b GlyR glycine</t>
+  </si>
+  <si>
+    <t>glycine</t>
+  </si>
+  <si>
+    <t>A3F</t>
+  </si>
+  <si>
+    <t>A2F</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>A3R</t>
+  </si>
+  <si>
+    <t>A3FS</t>
+  </si>
+  <si>
+    <t>A2FS</t>
+  </si>
+  <si>
+    <t>AFS</t>
+  </si>
+  <si>
+    <t>gamma3</t>
+  </si>
+  <si>
+    <t>delta3</t>
+  </si>
+  <si>
+    <t>gamma2</t>
+  </si>
+  <si>
+    <t>delta2</t>
+  </si>
+  <si>
+    <t>gamma1</t>
+  </si>
+  <si>
+    <t>delta1</t>
+  </si>
+  <si>
+    <t>3kfm3</t>
+  </si>
+  <si>
+    <t>kfp3</t>
+  </si>
+  <si>
+    <t>2kfm2</t>
+  </si>
+  <si>
+    <t>2kfp2</t>
+  </si>
+  <si>
+    <t>3km3</t>
+  </si>
+  <si>
+    <t>kp3</t>
+  </si>
+  <si>
+    <t>2km2</t>
+  </si>
+  <si>
+    <t>2kp2</t>
+  </si>
+  <si>
+    <t>km1</t>
+  </si>
+  <si>
+    <t>3kp1</t>
+  </si>
+  <si>
+    <t>alpha3</t>
+  </si>
+  <si>
+    <t>beta3</t>
+  </si>
+  <si>
+    <t>Lape2008 heteromericGlyR - taurine</t>
+  </si>
+  <si>
+    <t>Lape a1b GlyR taurine</t>
+  </si>
+  <si>
+    <t>3 site flip taurine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +335,18 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF657B83"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF268BD2"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -258,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -267,12 +377,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -291,9 +409,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -331,7 +449,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -437,7 +555,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -579,7 +697,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -793,7 +911,6 @@
         <v>10000000</v>
       </c>
       <c r="I12" s="5"/>
-      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -818,7 +935,6 @@
         <v>10000000</v>
       </c>
       <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -843,7 +959,6 @@
         <v>10000000</v>
       </c>
       <c r="I14" s="5"/>
-      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -868,7 +983,7 @@
         <v>10000000</v>
       </c>
       <c r="I15" s="5"/>
-      <c r="J15" s="7"/>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -893,7 +1008,7 @@
         <v>10000000</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="8"/>
+      <c r="J16" s="7"/>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -921,7 +1036,7 @@
       <c r="I17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="7">
         <v>2</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -956,10 +1071,10 @@
       <c r="I18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="7">
         <v>2</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="K18" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -991,7 +1106,7 @@
       <c r="I19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="8"/>
+      <c r="J19" s="7"/>
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1020,7 +1135,7 @@
         <v>10000000</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="8"/>
+      <c r="J20" s="7"/>
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1048,7 +1163,7 @@
       <c r="I21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="7">
         <v>1</v>
       </c>
       <c r="K21" s="1"/>
@@ -1119,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE59CC13-DA1A-4026-A931-51508FFF0962}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1291,7 +1406,7 @@
       <c r="D13" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>1</v>
       </c>
       <c r="G13" s="2">
@@ -1314,7 +1429,7 @@
       <c r="D14" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>1</v>
       </c>
       <c r="G14" s="2">
@@ -1337,7 +1452,7 @@
       <c r="D15" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>1</v>
       </c>
       <c r="G15" s="2">
@@ -1360,7 +1475,7 @@
       <c r="D16" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>1</v>
       </c>
       <c r="G16" s="2">
@@ -1383,7 +1498,7 @@
       <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="8">
         <v>1</v>
       </c>
       <c r="G17" s="2">
@@ -1406,7 +1521,7 @@
       <c r="D18" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>1</v>
       </c>
       <c r="G18" s="2">
@@ -1429,7 +1544,7 @@
       <c r="D19" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>1</v>
       </c>
       <c r="G19" s="2">
@@ -1452,7 +1567,7 @@
       <c r="D20" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>1</v>
       </c>
       <c r="G20" s="2">
@@ -1475,7 +1590,7 @@
       <c r="D21" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <v>3</v>
       </c>
       <c r="G21" s="2">
@@ -1504,7 +1619,7 @@
       <c r="D22" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="8">
         <v>1</v>
       </c>
       <c r="G22" s="2">
@@ -1527,7 +1642,7 @@
       <c r="D23" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="8">
         <v>2</v>
       </c>
       <c r="G23" s="2">
@@ -1556,7 +1671,7 @@
       <c r="D24" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>1</v>
       </c>
       <c r="G24" s="2">
@@ -1579,7 +1694,7 @@
       <c r="D25" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="8">
         <v>1</v>
       </c>
       <c r="G25" s="2">
@@ -1602,7 +1717,7 @@
       <c r="D26" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="8">
         <v>1</v>
       </c>
       <c r="G26" s="2">
@@ -1639,6 +1754,1735 @@
       <c r="D28">
         <v>1</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0866B230-C51A-46FB-98BD-A7CFA322EFCF}">
+  <dimension ref="A1:L48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" s="11"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6E-11</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6E-11</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6E-11</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="L16" s="10"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18">
+        <v>3400</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H18" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19">
+        <v>4200</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H19" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="L19" s="10"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20">
+        <v>2100</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H20" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="L20" s="10"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21">
+        <v>28000</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H21" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="6"/>
+      <c r="L21" s="10"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22">
+        <v>7000</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H22" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="6"/>
+      <c r="L22" s="10"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23">
+        <v>129000</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H23" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="6"/>
+      <c r="L23" s="10"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24">
+        <v>900</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H24" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="6"/>
+      <c r="L24" s="10"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25">
+        <v>20900</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H25" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="6"/>
+      <c r="L25" s="10"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>18000</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H26" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="6"/>
+      <c r="L26" s="10"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27">
+        <v>6800</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H27" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="6"/>
+      <c r="L27" s="10"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28">
+        <v>29000</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H28" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="6"/>
+      <c r="L28" s="10"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29">
+        <v>180</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H29" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I29" s="5"/>
+      <c r="J29" s="6"/>
+      <c r="L29" s="10"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30">
+        <v>3600</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H30" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L30" s="10"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="2">
+        <v>150000000</v>
+      </c>
+      <c r="F31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H31" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="10"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2400</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H32" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="10"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="2">
+        <v>300000000</v>
+      </c>
+      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H33" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J33" s="7">
+        <v>2</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="L33" s="10"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="2">
+        <v>900</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H34" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J34" s="7">
+        <v>3</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L34" s="10"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="2">
+        <v>590000</v>
+      </c>
+      <c r="F35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H35" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="10"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="2">
+        <v>600</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H36" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J36" s="8">
+        <v>2</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L36" s="10"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1180000</v>
+      </c>
+      <c r="F37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H37" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J37" s="1">
+        <v>2</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L37" s="10"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="2">
+        <v>300</v>
+      </c>
+      <c r="G38" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H38" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="J38" s="1"/>
+      <c r="L38" s="10"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1770000</v>
+      </c>
+      <c r="F39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H39" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J39" s="1">
+        <v>3</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L39" s="11"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J48" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C4DEDC-E4E0-459C-987A-C2D52BFF921C}">
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L3" s="11"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6E-11</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6E-11</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15">
+        <v>1150</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H15" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16">
+        <v>250</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H16" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
+      <c r="L16" s="10"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17">
+        <v>14500</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H17" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="6"/>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18">
+        <v>133000</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H18" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="6"/>
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19">
+        <v>5170</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H19" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6"/>
+      <c r="L19" s="10"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20">
+        <v>740</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H20" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="6"/>
+      <c r="L20" s="10"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>739000</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H21" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="6"/>
+      <c r="L21" s="10"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22">
+        <v>96000</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H22" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="6"/>
+      <c r="L22" s="10"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23">
+        <v>3690</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H23" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="10"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2380000</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H24" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="10"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="2">
+        <v>660</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H25" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="7">
+        <v>3</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L25" s="10"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="2">
+        <v>220000</v>
+      </c>
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H26" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="10"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="2">
+        <v>440</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H27" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" s="8">
+        <v>2</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L27" s="10"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="2">
+        <v>440000</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H28" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="1">
+        <v>2</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L28" s="10"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="2">
+        <v>220</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H29" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="J29" s="1"/>
+      <c r="L29" s="10"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="2">
+        <v>650000</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="H30" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" s="1">
+        <v>3</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L30" s="11"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="J39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>